<commit_message>
Updating to OS Comm Items.
</commit_message>
<xml_diff>
--- a/PracticumProjectChecklist.xlsx
+++ b/PracticumProjectChecklist.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail</t>
+    <t>Rating</t>
   </si>
   <si>
     <t>Description</t>
@@ -40,7 +40,10 @@
     <t>Continuous Review</t>
   </si>
   <si>
-    <t>Verbose Error Messages Not in Use</t>
+    <t>Error Messages are Properly Handled</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
   <si>
     <t>Error messages should be short and generic. Do not show stack traces or informative messages to the user.</t>
@@ -52,7 +55,7 @@
     <t>Autocomplete Disabled on Sensitive Input Fields</t>
   </si>
   <si>
-    <t>Emails, password, challenge questions, and other sensitive information should have autocomplete=off.</t>
+    <t>Disable autocomplete on fields such as email, password, and security questions by setting autocomplete="off"</t>
   </si>
   <si>
     <t>https://www.w3schools.com/howto/howto_html_autocomplete_off.asp</t>
@@ -61,7 +64,10 @@
     <t>Sensitive Information is Masked</t>
   </si>
   <si>
-    <t>NPI should be masked to reduce shoulder surfing attacks.</t>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Sensitive Information should be masked to mitigate shoulder surfing attacks.</t>
   </si>
   <si>
     <t>https://labex.io/tutorials/javascript-mask-a-value-28489</t>
@@ -79,7 +85,7 @@
     <t>Unneccessary Methods are Disabled</t>
   </si>
   <si>
-    <t>Do not allow unsafe methods such as Trace or Connect on any endpoint. Disable delete, post, etc if not needed on the endpoint.</t>
+    <t>Do not allow unsafe methods such as Trace or Connect on any endpoint. Disable DELETE, POST, etc. if not needed on the endpoint.</t>
   </si>
   <si>
     <t>https://cyberwhite.co.uk/http-verbs-and-their-security-risks/</t>
@@ -88,13 +94,16 @@
     <t>HTTP Disabled</t>
   </si>
   <si>
-    <t>Force HTTPS connections.</t>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Enforce HTTPS for all connections.</t>
   </si>
   <si>
     <t>https://blog.matrixpost.net/redirect-from-http-to-https-using-the-iis-url-rewrite-module/</t>
   </si>
   <si>
-    <t>Response Headers:</t>
+    <t>Response Headers</t>
   </si>
   <si>
     <t>Content-Security-Policy</t>
@@ -137,7 +146,7 @@
     <t>HSTS Response Header</t>
   </si>
   <si>
-    <t xml:space="preserve">Strict-Transport-Security: max-age=63072000; includeSubDomains; preload   Only use preload if external app. </t>
+    <t>Use Strict-Transport-Security: max-age=63072000; includeSubDomains; preload. Only use preload if required.</t>
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Strict-Transport-Security</t>
@@ -146,7 +155,7 @@
     <t>Caching Headers</t>
   </si>
   <si>
-    <t>Cache-Control: no-store. More lax: Expires: 0, Cache-Control: no-cache</t>
+    <t>Use Cache-Control: no-store. Less strict controls: Expires: 0, Cache-Control: no-cache</t>
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Cache-Control
@@ -156,7 +165,10 @@
     <t>Information Leak Headers</t>
   </si>
   <si>
-    <t>Remove unneccessary headers, such as: Server, X-Powered-By,X-AspNet-Version.</t>
+    <t>Informational</t>
+  </si>
+  <si>
+    <t>Remove unneccessary response headers, such as: Server, X-Powered-By, X-AspNet-Version.</t>
   </si>
   <si>
     <t>https://support.waters.com/KB_Inf/Other/WKB202501_How_to_disable_the_Server_HTTP_header_in_Microsoft_IIS</t>
@@ -165,19 +177,19 @@
     <t>CORS Headers</t>
   </si>
   <si>
-    <t>Do not set Access-Control-Allow-Origin to wildcard or reflect arbitrary origins/subdomains.</t>
+    <t>Do not set Access-Control-Allow-Origin to wildcard or allow reflected arbitrary origins/subdomains.</t>
   </si>
   <si>
     <t>https://www.freecodecamp.org/news/exploiting-cors-guide-to-pentesting/#heading-exploitable-cors-cases</t>
   </si>
   <si>
-    <t>Cookies:</t>
+    <t>Cookies</t>
   </si>
   <si>
     <t>HttpOnly</t>
   </si>
   <si>
-    <t>Prevents JavaScript from accessing the cookies(an easy target for XSS attacks)</t>
+    <t>Prevents JavaScript from accessing the cookies, mitigating some XSS risks.</t>
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/HTTP/Reference/Headers/Set-Cookie</t>
@@ -186,13 +198,13 @@
     <t>Secure Flag</t>
   </si>
   <si>
-    <t>Prevents cookies from sending over HTTP.</t>
+    <t>Ensures cookies are only sent over HTTPS.</t>
   </si>
   <si>
     <t>SameSite Lax or Strict</t>
   </si>
   <si>
-    <t>SameSite cookies prevent cross-site attacks like CSRF. Lax: Cross-site requests will only send cookies in GET requests. Strict: Cookies will not send in any cross-site requests.</t>
+    <t>SameSite cookies control cross-site request behavior to prevent CSRF. Lax: Cross-site requests will only send cookies in GET requests. Strict: Cookies will not send in any cross-site requests.</t>
   </si>
   <si>
     <r>
@@ -226,31 +238,65 @@
     <t>Narrow Domain</t>
   </si>
   <si>
-    <t>Sensitive/session cookies must have the domain set to the subdomain when applicable.</t>
+    <t>Sensitive/session cookies should have a narrow domain, set to a specific subdomain when applicable.</t>
   </si>
   <si>
     <t>https://developer.mozilla.org/en-US/docs/Web/Security/Practical_implementation_guides/Cookies</t>
   </si>
   <si>
-    <t>Injections/Payloads Required:</t>
+    <t>Injections/Payloads Required</t>
   </si>
   <si>
     <t>Cross-Site Scripting(XSS)</t>
   </si>
   <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>The application should encode user input when reflected to the UI.</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/Cross_Site_Scripting_Prevention_Cheat_Sheet.html
+https://learn.microsoft.com/en-us/aspnet/core/security/cross-site-scripting?view=aspnetcore-9.0</t>
+  </si>
+  <si>
     <t>SQL Injection</t>
   </si>
   <si>
+    <t>Use parameterized queries to prevent SQL injection via user input.</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/SQL_Injection_Prevention_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>SQL Injection on Login Page</t>
+  </si>
+  <si>
+    <t>Login pages must use parameterized queries.</t>
+  </si>
+  <si>
+    <t>https://unix.stackexchange.com/questions/391866/regex-for-password-restricting-special-characters</t>
+  </si>
+  <si>
     <t>Directory Traversal</t>
   </si>
   <si>
+    <t>User Input must be validated and canonicalized before being used to retrieve files from the server.</t>
+  </si>
+  <si>
+    <t>https://portswigger.net/web-security/file-path-traversal</t>
+  </si>
+  <si>
     <t>OS Command Injection</t>
   </si>
   <si>
-    <t>SQL Injection on Login Page</t>
-  </si>
-  <si>
-    <t>Login Page:</t>
+    <t>Do not place user input directly into system command executions.</t>
+  </si>
+  <si>
+    <t>https://developers.redhat.com/articles/2023/03/29/4-essentials-prevent-os-command-injection-attacks#4_ways_to_prevent_os_command_injection_attacks</t>
+  </si>
+  <si>
+    <t>Login Page</t>
   </si>
   <si>
     <t>Weak Passwords Not Allowed</t>
@@ -262,13 +308,13 @@
     <t>Account Lockout Enabled</t>
   </si>
   <si>
-    <t>Multi-Factor Authentication</t>
-  </si>
-  <si>
-    <t>Session Management:</t>
-  </si>
-  <si>
-    <t>Session Fixation</t>
+    <t>Multi-Factor Authentication in Use</t>
+  </si>
+  <si>
+    <t>Session Management</t>
+  </si>
+  <si>
+    <t>Session Fixation Not Possible</t>
   </si>
   <si>
     <t>Session dies after X minutes</t>
@@ -293,13 +339,42 @@
   </si>
   <si>
     <t>Vertical Privilege Escalation-MFLAC</t>
+  </si>
+  <si>
+    <t>The risk ratings were generated by reviewing average ratings of CVEs for the corresponding CWE.</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">For a more accurate risk rating, please use the following calculator: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://nvd.nist.gov/vuln-metrics/cvss/v4-calculator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Discuss: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://owasp.org/www-community/OWASP_Risk_Rating_Methodology</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -361,6 +436,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -388,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -407,6 +486,9 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -419,41 +501,47 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,8 +760,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="40.13"/>
-    <col customWidth="1" min="2" max="2" width="5.75"/>
-    <col customWidth="1" min="3" max="3" width="5.63"/>
+    <col customWidth="1" min="2" max="2" width="6.13"/>
+    <col customWidth="1" min="3" max="3" width="11.0"/>
     <col customWidth="1" min="4" max="4" width="94.63"/>
     <col customWidth="1" min="5" max="5" width="67.25"/>
   </cols>
@@ -701,13 +789,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -715,351 +803,486 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>14</v>
       </c>
+      <c r="E5" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="9"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>36</v>
+      <c r="A14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>46</v>
+      <c r="A20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>51</v>
+      <c r="A21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>54</v>
+      <c r="A22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>57</v>
-      </c>
+      <c r="A23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="s">
-        <v>58</v>
+      <c r="A26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13" t="s">
-        <v>59</v>
+      <c r="A27" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="8" t="s">
-        <v>60</v>
+      <c r="A28" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>61</v>
+        <v>73</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="8" t="s">
-        <v>63</v>
+      <c r="A30" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="8"/>
+      <c r="A32" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="8"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="43">
-      <c r="A43" s="8" t="s">
-        <v>73</v>
-      </c>
+      <c r="A43" s="9"/>
     </row>
     <row r="44">
-      <c r="A44" s="8"/>
+      <c r="A44" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>74</v>
+      <c r="A45" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="21" t="s">
-        <v>75</v>
+      <c r="A46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="s">
-        <v>76</v>
+      <c r="A47" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="7" t="s">
-        <v>78</v>
+      <c r="A48" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="24" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1303,14 @@
     <hyperlink r:id="rId14" ref="E21"/>
     <hyperlink r:id="rId15" ref="E22"/>
     <hyperlink r:id="rId16" ref="E23"/>
+    <hyperlink r:id="rId17" ref="E26"/>
+    <hyperlink r:id="rId18" ref="E27"/>
+    <hyperlink r:id="rId19" ref="E28"/>
+    <hyperlink r:id="rId20" ref="E29"/>
+    <hyperlink r:id="rId21" location="4_ways_to_prevent_os_command_injection_attacks" ref="E30"/>
+    <hyperlink r:id="rId22" ref="A51"/>
+    <hyperlink r:id="rId23" ref="A52"/>
   </hyperlinks>
-  <drawing r:id="rId17"/>
+  <drawing r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final checklist items updated.
</commit_message>
<xml_diff>
--- a/PracticumProjectChecklist.xlsx
+++ b/PracticumProjectChecklist.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="121">
   <si>
     <t>Pass</t>
   </si>
@@ -402,13 +402,93 @@
     <t>Clickjacking</t>
   </si>
   <si>
-    <t>File upload</t>
+    <t>Use X-Frame-Options: DENY or frame-ancestors CSP directive to prevent clickjacking attacks.</t>
+  </si>
+  <si>
+    <t>https://cheatsheetseries.owasp.org/cheatsheets/Clickjacking_Defense_Cheat_Sheet.html</t>
+  </si>
+  <si>
+    <t>File Upload</t>
+  </si>
+  <si>
+    <t>Only allow necessary file types. Virus scan each file and rename upon upload.</t>
+  </si>
+  <si>
+    <t>https://github.com/dilaouid/shitshit/blob/main/backend-good-practices-security/FILE_UPLOAD.md</t>
   </si>
   <si>
     <t>Horizontal Privilege Escalation-IDOR</t>
   </si>
   <si>
+    <t>Ensure users cannot access resources that belong to other users.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">High level: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://purplesec.us/learn/privilege-escalation-attacks/</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+In depth: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://portswigger.net/web-security/access-control</t>
+    </r>
+  </si>
+  <si>
     <t>Vertical Privilege Escalation-MFLAC</t>
+  </si>
+  <si>
+    <t>Ensure unauthorized users cannot execute privileged functionality.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://owasp.org/www-project-web-security-testing-guide/latest/4-Web_Application_Security_Testing/05-Authorization_Testing/03-Testing_for_Privilege_Escalation</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://cheatsheetseries.owasp.org/cheatsheets/Authorization_Cheat_Sheet.html</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
   <si>
     <t>The risk ratings were generated by reviewing average ratings of CVEs for the corresponding CWE.</t>
@@ -444,7 +524,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -470,7 +550,7 @@
     <font>
       <sz val="9.0"/>
       <color rgb="FF000000"/>
-      <name val="Menlo"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -525,6 +605,16 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -552,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -639,6 +729,12 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,7 +955,7 @@
     <col customWidth="1" min="1" max="1" width="37.0"/>
     <col customWidth="1" min="2" max="2" width="5.38"/>
     <col customWidth="1" min="3" max="3" width="11.0"/>
-    <col customWidth="1" min="4" max="4" width="82.25"/>
+    <col customWidth="1" min="4" max="4" width="82.13"/>
     <col customWidth="1" min="5" max="5" width="78.5"/>
   </cols>
   <sheetData>
@@ -1402,53 +1498,73 @@
       <c r="C45" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="17"/>
+      <c r="D45" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="17"/>
+      <c r="D46" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="17"/>
+      <c r="D47" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E48" s="17"/>
+      <c r="D48" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="49">
       <c r="E49" s="17"/>
     </row>
     <row r="50">
       <c r="A50" s="8" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E50" s="17"/>
     </row>
     <row r="51">
       <c r="A51" s="27" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E51" s="17"/>
     </row>
     <row r="52">
       <c r="A52" s="27" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E52" s="17"/>
     </row>
@@ -4333,9 +4449,13 @@
     <hyperlink r:id="rId27" ref="E40"/>
     <hyperlink r:id="rId28" ref="E41"/>
     <hyperlink r:id="rId29" ref="E42"/>
-    <hyperlink r:id="rId30" ref="A51"/>
-    <hyperlink r:id="rId31" ref="A52"/>
+    <hyperlink r:id="rId30" ref="E45"/>
+    <hyperlink r:id="rId31" ref="E46"/>
+    <hyperlink r:id="rId32" ref="E47"/>
+    <hyperlink r:id="rId33" ref="E48"/>
+    <hyperlink r:id="rId34" ref="A51"/>
+    <hyperlink r:id="rId35" ref="A52"/>
   </hyperlinks>
-  <drawing r:id="rId32"/>
+  <drawing r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>